<commit_message>
updated information gain comparison
</commit_message>
<xml_diff>
--- a/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
+++ b/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="54">
   <si>
     <t>Team Number:</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>File1-Leaf Failure</t>
-  </si>
-  <si>
-    <t>Part 1-beginning</t>
   </si>
   <si>
     <t>Part 2-at mid(10,000 rows</t>
@@ -5035,10 +5032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH49"/>
+  <dimension ref="A1:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5514,71 +5511,59 @@
         <v>47</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="26">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="E19" s="26">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F19" s="26">
-        <f t="shared" ref="F19:P19" si="2">1/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="I19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="J19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.59</v>
       </c>
       <c r="K19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="L19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="M19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="N19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="O19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="P19" s="26">
-        <f t="shared" si="2"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.01</v>
       </c>
       <c r="R19" s="3">
-        <f t="shared" ref="R19:R21" si="3">SUM(D19:P19)</f>
-        <v>0.99999999999999956</v>
+        <f t="shared" ref="R19:R20" si="2">SUM(D19:P19)</f>
+        <v>1</v>
       </c>
       <c r="T19" s="11">
-        <f>SUM(V19:AH19)</f>
-        <v>0</v>
+        <f t="shared" ref="T19:T20" si="3">SUM(V19:AH19)</f>
+        <v>3.8237493603082728</v>
       </c>
       <c r="U19" s="13"/>
       <c r="V19">
-        <f t="shared" ref="V19:AH21" si="4">LOG(D19/D$3, 2)*D$23</f>
+        <f t="shared" ref="V19:AH20" si="4">LOG(D19/D$3, 2)*D$22</f>
         <v>0</v>
       </c>
       <c r="W19">
@@ -5603,7 +5588,7 @@
       </c>
       <c r="AB19">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.8237493603082728</v>
       </c>
       <c r="AC19">
         <f t="shared" si="4"/>
@@ -5635,11 +5620,11 @@
         <v>48</v>
       </c>
       <c r="B20" s="1">
-        <v>112</v>
+        <v>233</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="26">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="E20" s="26">
         <v>0.01</v>
@@ -5657,7 +5642,7 @@
         <v>0.01</v>
       </c>
       <c r="J20" s="26">
-        <v>0.59</v>
+        <v>0.88</v>
       </c>
       <c r="K20" s="26">
         <v>0.01</v>
@@ -5678,12 +5663,12 @@
         <v>0.01</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T20" s="11">
-        <f t="shared" ref="T20:T21" si="5">SUM(V20:AH20)</f>
-        <v>3.8237493603082728</v>
+        <f t="shared" si="3"/>
+        <v>4.400537929583729</v>
       </c>
       <c r="U20" s="13"/>
       <c r="V20">
@@ -5712,7 +5697,7 @@
       </c>
       <c r="AB20">
         <f t="shared" si="4"/>
-        <v>3.8237493603082728</v>
+        <v>4.400537929583729</v>
       </c>
       <c r="AC20">
         <f t="shared" si="4"/>
@@ -5739,1027 +5724,742 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="18.75">
-      <c r="A21" t="s">
+    <row r="21" spans="1:34">
+      <c r="D21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1">
-        <v>233</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="E21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="F21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="G21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="H21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="I21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="J21" s="26">
+      <c r="R21" s="2"/>
+      <c r="T21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="18.75">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <f>SUM(D22:P22)</f>
+        <v>1</v>
+      </c>
+      <c r="T22" s="14">
+        <f>AVERAGE(T19:T20)</f>
+        <v>4.1121436449460012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" ht="18.75">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="R23" s="3"/>
+      <c r="T23" s="17"/>
+    </row>
+    <row r="24" spans="1:34">
+      <c r="A24" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="18.75">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="21">
+        <v>112</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21">
         <v>0.88</v>
       </c>
-      <c r="K21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="L21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="M21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="N21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="O21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="P21" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="R21" s="3">
-        <f t="shared" si="3"/>
+      <c r="E25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="G25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="I25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="J25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="K25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="L25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="M25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="N25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="O25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="P25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="R25" s="3">
+        <f t="shared" ref="R25:R26" si="5">SUM(D25:P25)</f>
         <v>1</v>
       </c>
-      <c r="T21" s="11">
-        <f t="shared" si="5"/>
-        <v>4.400537929583729</v>
-      </c>
-      <c r="U21" s="13"/>
-      <c r="V21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="4"/>
-        <v>4.400537929583729</v>
-      </c>
-      <c r="AC21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AF21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AG21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AH21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34">
-      <c r="D22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="R22" s="2"/>
-      <c r="T22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" ht="18.75">
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <v>1</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3">
-        <f>SUM(D23:P23)</f>
-        <v>1</v>
-      </c>
-      <c r="T23" s="14">
-        <f>AVERAGE(T19:T21)</f>
-        <v>2.7414290966306676</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" ht="18.75">
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="R24" s="3"/>
-      <c r="T24" s="17"/>
-    </row>
-    <row r="25" spans="1:34">
-      <c r="A25" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
+      <c r="T25" s="11">
+        <f t="shared" ref="T25:T26" si="6">SUM(V25:AH25)</f>
+        <v>0.81557542886257262</v>
+      </c>
+      <c r="U25" s="13"/>
+      <c r="V25">
+        <f t="shared" ref="V25:AH26" si="7">LOG(D25/D$3, 2)*D$28</f>
+        <v>0.81557542886257262</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="18.75">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="E26" s="26">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F26" s="26">
-        <f t="shared" ref="F26:P26" si="6">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P26" s="26">
-        <f t="shared" si="6"/>
-        <v>4.1666666666666664E-2</v>
+        <v>48</v>
+      </c>
+      <c r="B26" s="21">
+        <v>245</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="G26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="I26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="J26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="K26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="L26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="M26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="N26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="O26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="P26" s="23">
+        <v>0.01</v>
       </c>
       <c r="R26" s="3">
-        <f t="shared" ref="R26:R28" si="7">SUM(D26:P26)</f>
-        <v>0.99999999999999956</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="T26" s="11">
-        <f>SUM(V26:AH26)</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.81557542886257262</v>
       </c>
       <c r="U26" s="13"/>
       <c r="V26">
-        <f t="shared" ref="V26:AH28" si="8">LOG(D26/D$3, 2)*D$30</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>0.81557542886257262</v>
       </c>
       <c r="W26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34">
+      <c r="D27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="T27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" ht="18.75">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <f>SUM(D28:P28)</f>
+        <v>1</v>
+      </c>
+      <c r="T28" s="14">
+        <f>AVERAGE(T25:T26)</f>
+        <v>0.81557542886257262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
+      <c r="A29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" ht="18.75">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="1">
+        <v>113</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="P30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="R30" s="3">
+        <f t="shared" ref="R30:R31" si="8">SUM(D30:P30)</f>
+        <v>1</v>
+      </c>
+      <c r="T30" s="11">
+        <f t="shared" ref="T30:T31" si="9">SUM(V30:AH30)</f>
+        <v>3.9634741239748865</v>
+      </c>
+      <c r="U30" s="13"/>
+      <c r="V30">
+        <f t="shared" ref="V30:AH31" si="10">LOG(D30/D$3, 2)*D$33</f>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="10"/>
+        <v>3.9634741239748865</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" ht="18.75">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1">
+        <v>234</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="P31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="R31" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="X26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH26">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="18.75">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="21">
-        <v>112</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21">
-        <v>0.88</v>
-      </c>
-      <c r="E27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="F27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="G27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="H27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="I27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="J27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="K27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="L27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="M27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="N27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="O27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="P27" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="R27" s="3">
-        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="T27" s="11">
-        <f t="shared" ref="T27:T28" si="9">SUM(V27:AH27)</f>
-        <v>0.81557542886257262</v>
-      </c>
-      <c r="U27" s="13"/>
-      <c r="V27">
-        <f t="shared" si="8"/>
-        <v>0.81557542886257262</v>
-      </c>
-      <c r="W27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="X27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH27">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" ht="18.75">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="21">
-        <v>245</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21">
-        <v>0.88</v>
-      </c>
-      <c r="E28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="F28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="G28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="H28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="I28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="J28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="K28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="L28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="M28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="N28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="O28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="P28" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="R28" s="3">
-        <f t="shared" si="7"/>
+      <c r="T31" s="11">
+        <f t="shared" si="9"/>
+        <v>4.0703893278913981</v>
+      </c>
+      <c r="U31" s="13"/>
+      <c r="V31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="10"/>
+        <v>4.0703893278913981</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34">
+      <c r="D32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="T32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="18.75">
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
         <v>1</v>
       </c>
-      <c r="T28" s="11">
-        <f t="shared" si="9"/>
-        <v>0.81557542886257262</v>
-      </c>
-      <c r="U28" s="13"/>
-      <c r="V28">
-        <f t="shared" si="8"/>
-        <v>0.81557542886257262</v>
-      </c>
-      <c r="W28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:34">
-      <c r="D29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="T29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" ht="18.75">
-      <c r="D30" s="1">
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <f>SUM(D33:P33)</f>
         <v>1</v>
       </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1">
-        <v>0</v>
-      </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1">
-        <v>0</v>
-      </c>
-      <c r="M30" s="1">
-        <v>0</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1">
-        <v>0</v>
-      </c>
-      <c r="R30" s="3">
-        <f>SUM(D30:P30)</f>
-        <v>1</v>
-      </c>
-      <c r="T30" s="14">
-        <f>AVERAGE(T26:T28)</f>
-        <v>0.54371695257504837</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34">
-      <c r="A31" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" ht="18.75">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="26">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F32" s="26">
-        <f t="shared" ref="F32:P32" si="10">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P32" s="26">
-        <f t="shared" si="10"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R32" s="3">
-        <f t="shared" ref="R32:R34" si="11">SUM(D32:P32)</f>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T32" s="11">
-        <f>SUM(V32:AH32)</f>
-        <v>0</v>
-      </c>
-      <c r="U32" s="13"/>
-      <c r="V32">
-        <f t="shared" ref="V32:AH34" si="12">LOG(D32/D$3, 2)*D$36</f>
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AB32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AH32">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:34" ht="18.75">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="1">
-        <v>113</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="G33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="I33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="K33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="L33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="N33" s="4">
-        <v>0.65</v>
-      </c>
-      <c r="O33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="P33" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="R33" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="T33" s="11">
-        <f t="shared" ref="T33:T34" si="13">SUM(V33:AH33)</f>
-        <v>2.9045804349213178</v>
-      </c>
-      <c r="U33" s="13"/>
-      <c r="V33">
-        <f t="shared" si="12"/>
-        <v>-1.0588936890535685</v>
-      </c>
-      <c r="W33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AB33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF33">
-        <f t="shared" si="12"/>
-        <v>3.9634741239748865</v>
-      </c>
-      <c r="AG33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AH33">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:34" ht="18.75">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="1">
-        <v>234</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="H34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="I34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="J34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="K34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="L34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="N34" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="O34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="P34" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="R34" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="T34" s="11">
-        <f t="shared" si="13"/>
-        <v>2.6744606515602589</v>
-      </c>
-      <c r="U34" s="13"/>
-      <c r="V34">
-        <f t="shared" si="12"/>
-        <v>-1.3959286763311392</v>
-      </c>
-      <c r="W34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AB34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF34">
-        <f t="shared" si="12"/>
-        <v>4.0703893278913981</v>
-      </c>
-      <c r="AG34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AH34">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34">
-      <c r="D35" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="T35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34" ht="18.75">
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
-      <c r="J36" s="1">
-        <v>0</v>
-      </c>
-      <c r="K36" s="1">
-        <v>0</v>
-      </c>
-      <c r="L36" s="1">
-        <v>0</v>
-      </c>
-      <c r="M36" s="1">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1">
-        <v>1</v>
-      </c>
-      <c r="O36" s="1">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1">
-        <v>0</v>
-      </c>
-      <c r="R36" s="3">
-        <f>SUM(D36:P36)</f>
-        <v>2</v>
-      </c>
-      <c r="T36" s="14">
-        <f>AVERAGE(T32:T34)</f>
-        <v>1.8596803621605256</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34">
-      <c r="A37" s="15"/>
-    </row>
-    <row r="38" spans="1:34" ht="18.75">
+      <c r="T33" s="14">
+        <f>AVERAGE(T30:T31)</f>
+        <v>4.0169317259331425</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" s="15"/>
+    </row>
+    <row r="35" spans="1:21" ht="18.75">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+    </row>
+    <row r="36" spans="1:21" ht="18.75">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+    </row>
+    <row r="37" spans="1:21" ht="18.75">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+    </row>
+    <row r="38" spans="1:21" ht="18.75">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
       <c r="Q38" s="2"/>
@@ -6768,64 +6468,64 @@
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
     </row>
-    <row r="39" spans="1:34" ht="18.75">
-      <c r="B39" s="2"/>
+    <row r="39" spans="1:21" ht="18.75">
+      <c r="B39" s="19"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="8"/>
       <c r="S39" s="2"/>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
     </row>
-    <row r="40" spans="1:34" ht="18.75">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
+    <row r="40" spans="1:21" ht="18.75">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="22"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="8"/>
       <c r="S40" s="2"/>
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
     </row>
-    <row r="41" spans="1:34" ht="18.75">
+    <row r="41" spans="1:21" ht="18.75">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="2"/>
@@ -6834,98 +6534,98 @@
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
     </row>
-    <row r="42" spans="1:34" ht="18.75">
-      <c r="B42" s="19"/>
+    <row r="42" spans="1:21" ht="18.75">
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="8"/>
       <c r="S42" s="2"/>
       <c r="T42" s="13"/>
       <c r="U42" s="13"/>
     </row>
-    <row r="43" spans="1:34" ht="18.75">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="28"/>
-      <c r="P43" s="22"/>
+    <row r="43" spans="1:21">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="8"/>
+      <c r="R43" s="2"/>
       <c r="S43" s="2"/>
-      <c r="T43" s="13"/>
-      <c r="U43" s="13"/>
-    </row>
-    <row r="44" spans="1:34" ht="18.75">
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+    </row>
+    <row r="44" spans="1:21" ht="18.75">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="8"/>
       <c r="S44" s="2"/>
-      <c r="T44" s="13"/>
-      <c r="U44" s="13"/>
-    </row>
-    <row r="45" spans="1:34" ht="18.75">
+      <c r="T44" s="17"/>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="1:21">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
-      <c r="R45" s="8"/>
+      <c r="R45" s="2"/>
       <c r="S45" s="2"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="13"/>
-    </row>
-    <row r="46" spans="1:34">
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:21">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="29"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -6944,72 +6644,6 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
     </row>
-    <row r="47" spans="1:34" ht="18.75">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="17"/>
-      <c r="U47" s="2"/>
-    </row>
-    <row r="48" spans="1:34">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-    </row>
-    <row r="49" spans="2:21">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
uploading documentation for the project
</commit_message>
<xml_diff>
--- a/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
+++ b/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="60" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1680" yWindow="60" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Set" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="55">
   <si>
     <t>Team Number:</t>
   </si>
@@ -183,6 +183,9 @@
   <si>
     <t>outcome vector for File 3</t>
   </si>
+  <si>
+    <t>Average after certainty of outcome</t>
+  </si>
 </sst>
 </file>
 
@@ -276,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -305,6 +308,19 @@
       </left>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -354,7 +370,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -385,6 +401,8 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -763,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH62"/>
+  <dimension ref="A1:AH63"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2161,13 +2179,13 @@
       <c r="M28" s="1">
         <v>0</v>
       </c>
-      <c r="N28" s="1">
-        <v>0</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1">
+      <c r="N28" s="30">
+        <v>0</v>
+      </c>
+      <c r="O28" s="30">
+        <v>0</v>
+      </c>
+      <c r="P28" s="30">
         <v>1</v>
       </c>
       <c r="R28" s="3">
@@ -2190,11 +2208,17 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="N29" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
       <c r="R29" s="3"/>
-      <c r="T29" s="17"/>
+      <c r="T29" s="14">
+        <f>AVERAGE(T23:T26)</f>
+        <v>3.3866230880890056</v>
+      </c>
     </row>
     <row r="30" spans="1:34">
       <c r="A30" s="15" t="s">
@@ -5017,6 +5041,19 @@
       <c r="T62" s="14">
         <f>AVERAGE(T53:T60)</f>
         <v>1.3077815648238174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34" ht="18.75">
+      <c r="N63" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="O63" s="31"/>
+      <c r="P63" s="31"/>
+      <c r="Q63" s="31"/>
+      <c r="R63" s="3"/>
+      <c r="T63" s="14">
+        <f>AVERAGE(T57:T60)</f>
+        <v>4.2006992324196677</v>
       </c>
     </row>
   </sheetData>
@@ -5034,8 +5071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
post presentation CaseE analysis
</commit_message>
<xml_diff>
--- a/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
+++ b/Documentation/Information_Gain_Comparison_Test_and_Training.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="60" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="60" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Set" sheetId="2" r:id="rId1"/>
     <sheet name="Training Set" sheetId="3" r:id="rId2"/>
+    <sheet name="CaseE" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="56">
   <si>
     <t>Team Number:</t>
   </si>
@@ -185,6 +186,9 @@
   </si>
   <si>
     <t>Average after certainty of outcome</t>
+  </si>
+  <si>
+    <t>Test Case E</t>
   </si>
 </sst>
 </file>
@@ -783,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19:T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6684,4 +6688,462 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A7:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="1:20">
+      <c r="A7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="18.75">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.24538352999999999</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L8" s="4">
+        <v>2.776207E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0.24307604999999999</v>
+      </c>
+      <c r="O8" s="4">
+        <v>4.4109620000000002E-2</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0.35966872999999999</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" ref="R8:R15" si="0">SUM(D8:P8)</f>
+        <v>1</v>
+      </c>
+      <c r="T8" s="11">
+        <f>SUM(V8:AH8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="18.75">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.25891874999999998</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.16922271999999999</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2.024405E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.18280083999999999</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.28881363999999998</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T9" s="11">
+        <f t="shared" ref="T9:T15" si="1">SUM(V9:AH9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="18.75">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.21894768000000001</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.24517025000000001</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0.15536422999999999</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0.29051782999999998</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999999000000006</v>
+      </c>
+      <c r="T10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="18.75">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.15336805000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M11" s="4">
+        <v>9.2121540000000002E-2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.29055585</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.37395455999999999</v>
+      </c>
+      <c r="R11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="18.75">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="R12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="18.75">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="20"/>
+      <c r="R13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18.75">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="20"/>
+      <c r="R14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="18.75">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="20"/>
+      <c r="R15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="T16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" ht="18.75">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="30">
+        <v>0</v>
+      </c>
+      <c r="O17" s="30">
+        <v>0</v>
+      </c>
+      <c r="P17" s="30">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
+        <f>SUM(D17:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="14">
+        <f>AVERAGE(T8:T15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="18.75">
+      <c r="R18" s="3"/>
+      <c r="T18" s="14">
+        <f>AVERAGE(T12:T15)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>